<commit_message>
chore: update newsbot state
</commit_message>
<xml_diff>
--- a/historico_news.xlsx
+++ b/historico_news.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1053,6 +1053,383 @@
         <v>6</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:44:52</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>04/01 18:14</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>BBC Brasil</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Trump diz que sucessora de Maduro 'pagará preço muito alto' se 'não fizer o certo' na Venezuela; o que aconteceu até agora após ataque americano</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>https://www.bbc.com/portuguese/articles/cm2403jvm03o?at_medium=RSS&amp;at_campaign=rss</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>sc</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Ação militar e prisão de Maduro marcam auge de meses de e&lt;b&gt;sc&lt;/b&gt;alada de tensão entre os dois países. Maioria dos líderes da América Latina cond</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:44:53</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>04/01 18:00</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Folha de S.Paulo - Poder - Principal</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Republicanos se distancia de defesa da pena de morte feita por ministro</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>https://redir.folha.com.br/redir/online/poder/rss091/*https://www1.folha.uol.com.br/colunas/painel/2026/01/republicanos-se-distancia-de-defesa-da-pena-de-morte-feita-por-ministro.shtml</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>lula</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">orte para autores de feminicídio constrangeu integrantes do governo Luiz Inácio Lula da Silva e surpreendeu até integrantes de seu partido, o Republicanos. Segundo </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:44:54</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>04/01 18:00</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Folha de S.Paulo - Mercado - Principal</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>O que realmente merece planejamento financeiro</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://redir.folha.com.br/redir/online/mercado/rss091/*https://www1.folha.uol.com.br/blogs/de-grao-em-grao/2026/01/o-que-realmente-merece-planejamento-financeiro.shtml</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>sc</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>nsformar a vida em uma planilha cansativa. O efeito dessa confusão é curioso: di&lt;b&gt;sc&lt;/b&gt;ute-se demais o que é pequeno e decide-se de menos o que é grande.
+&amp;lt;a href=&amp;quot;http</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:44:55</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>04/01 15:00</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Folha de S.Paulo - Poder - Principal</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Pacheco trata indicação ao Supremo como página virada, dizem aliados</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://redir.folha.com.br/redir/online/poder/rss091/*https://www1.folha.uol.com.br/colunas/painel/2026/01/pacheco-trata-indicacao-ao-supremo-como-pagina-virada-dizem-aliados.shtml</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>senado</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>O ex-presidente do &amp;lt;a href=&amp;quot;https://www1.folha.uol.com.br/folha-topicos/&lt;b&gt;senado&lt;/b&gt;/&amp;quot;&amp;gt;Senado&amp;lt;/a&amp;gt; &amp;lt;a href=&amp;quot;https://www1.folha.uol.com.br/folha-topicos/rodrigo-pache</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:44:56</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>04/01 15:00</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Folha de S.Paulo - Mercado - Principal</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Portal da reforma tributária permite monitorar economia em tempo real</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://redir.folha.com.br/redir/online/mercado/rss091/*https://www1.folha.uol.com.br/blogs/que-imposto-e-esse/2026/01/portal-da-reforma-tributaria-permite-monitorar-economia-em-tempo-real.shtml</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>imposto</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>lha.com.br/redir/online/mercado/rss091/*https://www1.folha.uol.com.br/blogs/que-&lt;b&gt;imposto&lt;/b&gt;-e-esse/2026/01/portal-da-reforma-tributaria-permite-monitorar-economia-em-tempo</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:45:00</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>VEJA</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Itamaraty reforça na Celac preocupação com captura de Maduro na Venezuela</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>https://veja.abril.com.br/mundo/itamaraty-reforca-na-celac-preocupacao-com-captura-de-maduro-na-venezuela/</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>lula</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>tro das Relações Exteriores, Mauro Vieira reiterou posicionamento do presidente Lula em reunião com países latino-americanos e caribenhos</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:45:01</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>VEJA</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Forças armadas da Venezuela reconhecem Delcy Rodríguez como presidente interina</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>https://veja.abril.com.br/mundo/forcas-armadas-da-venezuela-reconhecem-delcy-rodriguez-como-presidente-interina/</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>câmara</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>O chefe do exército venezuelano referendou a decisão da Câmara Constitucional da Suprema Corte da Venezuela</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:45:02</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>VEJA</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Marco Rubio detalha exigências dos EUA para líderes da Venezuela após captura de Maduro</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>https://veja.abril.com.br/mundo/marco-rubio-detalha-exigencias-dos-eua-para-lideres-da-venezuela-apos-captura-de-maduro/</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>senado</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Senador americano estabelece condições sobre petróleo, tráfico e grupos armados para q</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:45:03</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>VEJA</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>‘O Agente Secreto’ vence o Critics Choice Awards 2026 de melhor filme internacional</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>https://veja.abril.com.br/cultura/o-agente-secreto-vence-o-critics-choice-awards-2026-de-melhor-filme-internacional/</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>sc</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>a é a primeira do Brasil a vencer a premiação, considerada &amp;#x27;termômetro&amp;#x27; para o O&lt;b&gt;sc&lt;/b&gt;ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>04/01/2026 22:45:03</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>VEJA</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>EUA não têm tropas em solo venezuelano, mas mantêm forças no Caribe, diz Pentágono</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://veja.abril.com.br/mundo/estados-unidos-nao-tem-tropas-em-solo-venezuelano-mas-mantem-forcas-no-caribe-diz-pentagono/</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>sc</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Forças americanas seguem em prontidão no Caribe, enquanto Trump não de&lt;b&gt;sc&lt;/b&gt;arta segunda operação militar em Caracas</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>